<commit_message>
📊 Update CSV + XLSX reports for master
</commit_message>
<xml_diff>
--- a/minio-report-tracker/xlxs/cellbox21.xlsx
+++ b/minio-report-tracker/xlxs/cellbox21.xlsx
@@ -722,7 +722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -774,7 +774,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -785,13 +785,13 @@
         <v>512</v>
       </c>
       <c r="D2" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
@@ -802,27 +802,27 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45844</v>
+        <v>45845</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>auth</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>512</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>493</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -830,27 +830,27 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45843</v>
+        <v>45846</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>idrepo</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>410</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -918,14 +918,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C7" t="n">
         <v>945</v>
       </c>
       <c r="D7" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -942,18 +942,18 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C8" t="n">
         <v>945</v>
       </c>
       <c r="D8" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -974,14 +974,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>945</v>
       </c>
       <c r="D9" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -998,11 +998,11 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>masterdata-tam</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -1054,30 +1054,30 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>pms</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>509</v>
+        <v>945</v>
       </c>
       <c r="D12" t="n">
-        <v>497</v>
+        <v>920</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H12" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1086,23 +1086,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>prereg</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>288</v>
+        <v>945</v>
       </c>
       <c r="D13" t="n">
-        <v>280</v>
+        <v>920</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1110,27 +1110,27 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>resident</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1126</v>
+        <v>945</v>
       </c>
       <c r="D14" t="n">
-        <v>1117</v>
+        <v>920</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1142,25 +1142,305 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>masterdata-kan</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>945</v>
+      </c>
+      <c r="D15" t="n">
+        <v>920</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
+      </c>
+      <c r="G15" t="n">
+        <v>15</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>masterdata-tam</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>945</v>
+      </c>
+      <c r="D16" t="n">
+        <v>920</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>masterdata-tam</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>945</v>
+      </c>
+      <c r="D17" t="n">
+        <v>920</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" t="n">
+        <v>15</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>pms</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>509</v>
+      </c>
+      <c r="D18" t="n">
+        <v>332</v>
+      </c>
+      <c r="E18" t="n">
+        <v>134</v>
+      </c>
+      <c r="F18" t="n">
+        <v>31</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>pms</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>509</v>
+      </c>
+      <c r="D19" t="n">
+        <v>497</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>288</v>
+      </c>
+      <c r="D20" t="n">
+        <v>280</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>288</v>
+      </c>
+      <c r="D21" t="n">
+        <v>280</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1106</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>20</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1117</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>9</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C24" t="n">
         <v>3</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D24" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>dsl</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" t="n">
         <v>2</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
         <v>1</v>
       </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>